<commit_message>
arunava: validations changed for landmark; user component & service added
</commit_message>
<xml_diff>
--- a/Documents/validations.xlsx
+++ b/Documents/validations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arunava_das\Documents\github\DemoProject\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAAE6A5-DF26-415F-ABAA-19DEC1D0492C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09043E6F-E004-4C58-A8F5-02DD7EDF21D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B9F080BF-8B07-46CF-B60C-E308A907F67E}"/>
   </bookViews>
@@ -463,103 +463,103 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -879,7 +879,7 @@
   <dimension ref="A2:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -900,79 +900,79 @@
   <sheetData>
     <row r="2" spans="1:14" ht="19.5" thickBot="1"/>
     <row r="3" spans="1:14">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="36"/>
+      <c r="E3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="14" t="s">
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="33" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="19.5" thickBot="1">
-      <c r="B4" s="26"/>
-      <c r="C4" s="29" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="29" t="s">
+      <c r="E4" s="34"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="30" t="s">
+      <c r="K4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="31" t="s">
+      <c r="M4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="17"/>
+      <c r="N4" s="34"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="15" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -981,36 +981,36 @@
       <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="22" t="s">
+      <c r="H5" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="26" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1025,22 +1025,22 @@
       <c r="G6" s="8">
         <v>0</v>
       </c>
-      <c r="H6" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="36" t="s">
+      <c r="H6" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="27" t="s">
         <v>22</v>
       </c>
       <c r="N6" s="10" t="s">
@@ -1048,13 +1048,13 @@
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="26" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="10" t="s">
@@ -1069,22 +1069,22 @@
       <c r="G7" s="8">
         <v>150</v>
       </c>
-      <c r="H7" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="36" t="s">
+      <c r="H7" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="27" t="s">
         <v>22</v>
       </c>
       <c r="N7" s="10" t="s">
@@ -1092,13 +1092,13 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="26">
         <v>2</v>
       </c>
       <c r="D8" s="10">
@@ -1113,22 +1113,22 @@
       <c r="G8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="28">
+      <c r="H8" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="19">
         <v>6</v>
       </c>
-      <c r="L8" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="36" t="s">
+      <c r="L8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="27" t="s">
         <v>22</v>
       </c>
       <c r="N8" s="10" t="s">
@@ -1136,13 +1136,13 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="8">
         <v>150</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="26">
         <v>50</v>
       </c>
       <c r="D9" s="10">
@@ -1157,39 +1157,39 @@
       <c r="G9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="26">
         <v>25</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="19">
         <v>25</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="19">
         <v>25</v>
       </c>
-      <c r="K9" s="28">
+      <c r="K9" s="19">
         <v>6</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="19">
         <v>100</v>
       </c>
-      <c r="M9" s="36">
-        <v>25</v>
+      <c r="M9" s="27">
+        <v>50</v>
       </c>
       <c r="N9" s="10">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="19.5" thickBot="1">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="18" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -1201,22 +1201,22 @@
       <c r="G10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="38" t="s">
+      <c r="I10" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="38" t="s">
+      <c r="J10" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="39" t="s">
+      <c r="K10" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="38" t="s">
+      <c r="L10" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="40" t="s">
+      <c r="M10" s="31" t="s">
         <v>26</v>
       </c>
       <c r="N10" s="3" t="s">
@@ -1224,8 +1224,8 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>

</xml_diff>

<commit_message>
frontend: validations changed for area; backend: login fixed; state field added
</commit_message>
<xml_diff>
--- a/Documents/validations.xlsx
+++ b/Documents/validations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arunava_das\Documents\github\DemoProject\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09043E6F-E004-4C58-A8F5-02DD7EDF21D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A008C25-A9C7-4FCF-A8C4-B02A7648062E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B9F080BF-8B07-46CF-B60C-E308A907F67E}"/>
   </bookViews>
@@ -113,13 +113,13 @@
     <t>"0-9"</t>
   </si>
   <si>
-    <t>"A-Z", "a-z", ",", "."</t>
-  </si>
-  <si>
     <t>"A-Z", "a-z", ","</t>
   </si>
   <si>
     <t>~</t>
+  </si>
+  <si>
+    <t>"A-Z", "a-z", ":", "-", ",", "."</t>
   </si>
 </sst>
 </file>
@@ -878,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162A151-250A-4A70-BFD9-E2ED4D6F3ABF}">
   <dimension ref="A2:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -893,7 +893,7 @@
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="11" max="11" width="8.140625" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" customWidth="1"/>
+    <col min="12" max="12" width="33.28515625" customWidth="1"/>
     <col min="13" max="13" width="21.5703125" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" customWidth="1"/>
   </cols>
@@ -1214,13 +1214,13 @@
         <v>24</v>
       </c>
       <c r="L10" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="31" t="s">
+      <c r="N10" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:14">

</xml_diff>